<commit_message>
complete analisis empirico DP
</commit_message>
<xml_diff>
--- a/resultados_cambio_tiempo.xlsx
+++ b/resultados_cambio_tiempo.xlsx
@@ -229,21 +229,7 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:trendlineType val="linear"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
-          </c:trendline>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="linear"/>
+            <c:trendlineType val="power"/>
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
@@ -1515,15 +1501,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>219074</xdr:colOff>
+      <xdr:colOff>9524</xdr:colOff>
       <xdr:row>47</xdr:row>
-      <xdr:rowOff>85724</xdr:rowOff>
+      <xdr:rowOff>19049</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>123825</xdr:colOff>
-      <xdr:row>67</xdr:row>
-      <xdr:rowOff>19049</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>142874</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1833,7 +1819,7 @@
   <dimension ref="A1:B60"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="O51" sqref="O51"/>
+      <selection activeCell="N56" sqref="N56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>